<commit_message>
fix pcb -5v riple
</commit_message>
<xml_diff>
--- a/Outputs/BOM/Bill of Materials-IOElectro_SimpleOscilloscope.xlsx
+++ b/Outputs/BOM/Bill of Materials-IOElectro_SimpleOscilloscope.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esmaeill\Documents\Altium\Projects\LAOS\Outputs\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\1008-simple-oscilloscope-hardware\Outputs\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="174">
   <si>
     <t>Comment</t>
   </si>
@@ -86,7 +86,7 @@
     <t>CAPACITOR ELECTROLYTIC 6.3x7mm</t>
   </si>
   <si>
-    <t>C8, C16</t>
+    <t>C8, C16, C36</t>
   </si>
   <si>
     <t>C-EL_6.5x7x2.5mm</t>
@@ -149,7 +149,7 @@
     <t>120pF</t>
   </si>
   <si>
-    <t>C30, C34</t>
+    <t>C30</t>
   </si>
   <si>
     <t>6.5-30pF</t>
@@ -173,6 +173,12 @@
     <t>C32</t>
   </si>
   <si>
+    <t>180pF</t>
+  </si>
+  <si>
+    <t>C34</t>
+  </si>
+  <si>
     <t>3V6</t>
   </si>
   <si>
@@ -221,7 +227,7 @@
     <t>FERRITE BEAD 0805 100R 100Mhz</t>
   </si>
   <si>
-    <t>FB1, FB2, FB3, FB4</t>
+    <t>FB1, FB3, FB4</t>
   </si>
   <si>
     <t>L-0805</t>
@@ -305,7 +311,7 @@
     <t>Axial Lead Inductors(Coils)For Signal Line 100uH 165mA</t>
   </si>
   <si>
-    <t>L1</t>
+    <t>L1, L2</t>
   </si>
   <si>
     <t>L-DIP_3x7mm_pin9mm</t>
@@ -383,7 +389,7 @@
     <t>150R</t>
   </si>
   <si>
-    <t>R6, R7</t>
+    <t>R6, R7, R13</t>
   </si>
   <si>
     <t>1.8M</t>
@@ -392,7 +398,7 @@
     <t>R8</t>
   </si>
   <si>
-    <t>R9, R13</t>
+    <t>R9</t>
   </si>
   <si>
     <t>3K</t>
@@ -895,7 +901,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1021,7 +1027,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
@@ -1161,7 +1167,7 @@
         <v>10</v>
       </c>
       <c r="F13" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1204,161 +1210,161 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="F16" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>54</v>
       </c>
       <c r="F17" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="E18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="F19" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="E20" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F20" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="F21" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F21" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="F22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
@@ -1366,159 +1372,159 @@
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="E24" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F24" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="F25" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F25" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="F26" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F26" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="F27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F27" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="E28" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F28" s="4">
+      <c r="D29" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F29" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F29" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="D30" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F30" s="4">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>114</v>
-      </c>
       <c r="E31" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F31" s="4">
         <v>3</v>
@@ -1529,19 +1535,19 @@
         <v>117</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>118</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F32" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1549,56 +1555,56 @@
         <v>119</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>120</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F33" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F34" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>123</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F35" s="4">
         <v>1</v>
@@ -1609,16 +1615,16 @@
         <v>124</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>125</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F36" s="4">
         <v>1</v>
@@ -1629,16 +1635,16 @@
         <v>126</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>127</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F37" s="4">
         <v>1</v>
@@ -1649,16 +1655,16 @@
         <v>128</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>129</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F38" s="4">
         <v>1</v>
@@ -1669,59 +1675,59 @@
         <v>130</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>131</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F39" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>132</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>133</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F40" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>135</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F41" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1729,96 +1735,96 @@
         <v>136</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>137</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F42" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>138</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F43" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F43" s="4">
+      <c r="B44" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F44" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C44" s="3" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="F44" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="D45" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="E45" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F45" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="F45" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="E46" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F46" s="4">
         <v>1</v>
@@ -1826,19 +1832,19 @@
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="D47" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="E47" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F47" s="4">
         <v>1</v>
@@ -1846,59 +1852,59 @@
     </row>
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="E48" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F48" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F48" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="E49" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F49" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="B50" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="F49" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="D50" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>168</v>
-      </c>
       <c r="E50" s="3" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F50" s="4">
         <v>1</v>
@@ -1906,27 +1912,47 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C51" s="3" t="s">
+      <c r="E51" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="F51" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="E51" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="F51" s="4">
+      <c r="C52" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F52" s="4">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="30" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="82" fitToHeight="0" orientation="portrait" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>